<commit_message>
execl data pushed to orch
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\REFrameworkDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85900122-2EE6-4833-8AC3-89890AC2D857}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D87E549-DFD9-4E32-A565-67390CA69E42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -127,6 +123,9 @@
   </si>
   <si>
     <t>Input description</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
   </si>
 </sst>
 </file>
@@ -504,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -552,10 +551,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -1629,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1653,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1675,7 +1674,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1686,7 +1685,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1697,7 +1696,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2687,7 +2686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2707,7 +2706,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2737,13 +2736,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>